<commit_message>
Trainee Detail - New Team
</commit_message>
<xml_diff>
--- a/src/test/java/file/test2.xlsx
+++ b/src/test/java/file/test2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Repositories\Project\g6\src\test\java\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C0A7B2-C2A5-421E-A15A-1E2EF7C3B5C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{910E1758-5DCB-4963-88E4-83E7A1CFEF7E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="44">
   <si>
     <t>Group no</t>
   </si>
@@ -45,15 +45,63 @@
     <t>Group 1</t>
   </si>
   <si>
+    <t>Project Code 1</t>
+  </si>
+  <si>
+    <t>Topic Code1</t>
+  </si>
+  <si>
+    <t>Topic Name1</t>
+  </si>
+  <si>
+    <t>Group Description1</t>
+  </si>
+  <si>
     <t>Group 2</t>
   </si>
   <si>
+    <t>Project Code 2</t>
+  </si>
+  <si>
+    <t>Topic Code2</t>
+  </si>
+  <si>
+    <t>Topic Name2</t>
+  </si>
+  <si>
+    <t>Group Description2</t>
+  </si>
+  <si>
     <t>Group 3</t>
   </si>
   <si>
+    <t>Project Code 3</t>
+  </si>
+  <si>
+    <t>Topic Code3</t>
+  </si>
+  <si>
+    <t>Topic Name3</t>
+  </si>
+  <si>
+    <t>Group Description3</t>
+  </si>
+  <si>
     <t>Group 4</t>
   </si>
   <si>
+    <t>Project Code 4</t>
+  </si>
+  <si>
+    <t>Topic Code4</t>
+  </si>
+  <si>
+    <t>Topic Name4</t>
+  </si>
+  <si>
+    <t>Group Description4</t>
+  </si>
+  <si>
     <t>Email</t>
   </si>
   <si>
@@ -106,58 +154,16 @@
   </si>
   <si>
     <t>Nguyen Van K</t>
-  </si>
-  <si>
-    <t>Project Code 1</t>
-  </si>
-  <si>
-    <t>Project Code 2</t>
-  </si>
-  <si>
-    <t>Project Code 3</t>
-  </si>
-  <si>
-    <t>Project Code 4</t>
-  </si>
-  <si>
-    <t>Topic Code 1</t>
-  </si>
-  <si>
-    <t>Topic Code 2</t>
-  </si>
-  <si>
-    <t>Topic Code 3</t>
-  </si>
-  <si>
-    <t>Topic Code 4</t>
-  </si>
-  <si>
-    <t>Topic Name 1</t>
-  </si>
-  <si>
-    <t>Topic Name 2</t>
-  </si>
-  <si>
-    <t>Topic Name 3</t>
-  </si>
-  <si>
-    <t>Topic Name 4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -521,7 +527,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{21A8127D-9BB9-4DF0-884E-225E3369D802}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E914CA5-D646-43AD-A638-09B4D91967F0}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -533,12 +539,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71D8A1EC-C191-40EE-9AC6-D2CA53099984}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5169B9AD-F240-42C0-8709-8D15BEEA2907}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -574,16 +578,16 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>36</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -591,19 +595,19 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D3" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>37</v>
+        <v>14</v>
       </c>
       <c r="F3" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -611,19 +615,19 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="F4" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -631,33 +635,32 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="E5" t="s">
-        <v>39</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2065FD9F-B585-4297-BE04-23BAAFA42A5D}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B0660A1-0C01-4B47-B0F5-0363841D2A77}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -672,83 +675,83 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>26</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>12</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2">
-        <v>1</v>
+        <v>31</v>
+      </c>
+      <c r="D2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>18</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4">
-        <v>1</v>
+        <v>35</v>
+      </c>
+      <c r="D4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>37</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
+        <v>39</v>
+      </c>
+      <c r="D6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -756,13 +759,13 @@
         <v>2</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
       <c r="D7" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -770,13 +773,13 @@
         <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8">
-        <v>1</v>
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>